<commit_message>
Add a backp panel design
</commit_message>
<xml_diff>
--- a/KIK01接続一覧表.xlsx
+++ b/KIK01接続一覧表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="105" windowWidth="22035" windowHeight="11445" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="22035" windowHeight="11445"/>
   </bookViews>
   <sheets>
     <sheet name="Nucleo" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="198">
   <si>
     <t>KIK01接続一覧表</t>
     <rPh sb="5" eb="7">
@@ -753,15 +753,55 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2017.12.05</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>CN6/CN8</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>CN5/CN9</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sync</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SyncGND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PWR_MON</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs_GND</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs_PWR</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs_Beat</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs_SyncIn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LEDs_SyncOut</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2017.12.12</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -895,7 +935,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -968,13 +1008,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1102,6 +1151,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1618,8 +1670,8 @@
   </sheetPr>
   <dimension ref="A1:X51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1634,7 +1686,8 @@
     <col min="11" max="11" width="3" customWidth="1"/>
     <col min="12" max="12" width="5.75" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3.125" customWidth="1"/>
-    <col min="15" max="16" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.625" customWidth="1"/>
     <col min="18" max="18" width="3.125" customWidth="1"/>
     <col min="19" max="20" width="10.375" bestFit="1" customWidth="1"/>
@@ -1647,7 +1700,7 @@
     </row>
     <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:24" s="5" customFormat="1">
@@ -1660,7 +1713,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="5" customFormat="1">
@@ -1910,6 +1963,12 @@
       <c r="C16" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="E16" t="s">
+        <v>187</v>
+      </c>
+      <c r="F16" t="s">
+        <v>188</v>
+      </c>
       <c r="G16" s="13"/>
       <c r="L16">
         <v>20</v>
@@ -1980,7 +2039,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" ht="14.25" thickBot="1">
       <c r="B19">
         <v>25</v>
       </c>
@@ -2001,7 +2060,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" ht="14.25" thickBot="1">
       <c r="B20">
         <v>27</v>
       </c>
@@ -2018,8 +2077,12 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
-      <c r="Q20" s="20" t="s">
+      <c r="Q20" s="43" t="s">
         <v>92</v>
+      </c>
+      <c r="R20" s="26"/>
+      <c r="S20" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -2128,7 +2191,7 @@
         <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:20" s="5" customFormat="1">
@@ -2245,6 +2308,13 @@
       <c r="M31" t="s">
         <v>58</v>
       </c>
+      <c r="N31" s="2"/>
+      <c r="O31" t="s">
+        <v>192</v>
+      </c>
+      <c r="P31" t="s">
+        <v>193</v>
+      </c>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
     </row>
@@ -2327,6 +2397,13 @@
       <c r="M34" t="s">
         <v>60</v>
       </c>
+      <c r="N34" s="7"/>
+      <c r="O34" t="s">
+        <v>192</v>
+      </c>
+      <c r="P34" t="s">
+        <v>194</v>
+      </c>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
     </row>
@@ -2350,6 +2427,13 @@
       <c r="M35" t="s">
         <v>61</v>
       </c>
+      <c r="N35" s="6"/>
+      <c r="O35" t="s">
+        <v>192</v>
+      </c>
+      <c r="P35" t="s">
+        <v>195</v>
+      </c>
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
     </row>
@@ -2373,6 +2457,13 @@
       <c r="M36" t="s">
         <v>62</v>
       </c>
+      <c r="N36" s="8"/>
+      <c r="O36" t="s">
+        <v>192</v>
+      </c>
+      <c r="P36" t="s">
+        <v>196</v>
+      </c>
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
     </row>
@@ -2434,10 +2525,10 @@
       </c>
       <c r="N38" s="29"/>
       <c r="O38" t="s">
-        <v>75</v>
+        <v>190</v>
       </c>
       <c r="P38" t="s">
-        <v>86</v>
+        <v>191</v>
       </c>
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
@@ -2632,6 +2723,13 @@
       </c>
       <c r="M44" s="3" t="s">
         <v>68</v>
+      </c>
+      <c r="N44" s="29"/>
+      <c r="O44" t="s">
+        <v>75</v>
+      </c>
+      <c r="P44" t="s">
+        <v>86</v>
       </c>
       <c r="Q44" s="13"/>
       <c r="R44" s="13"/>
@@ -2752,7 +2850,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add F446温度測定 Update KIK01接続一覧表
</commit_message>
<xml_diff>
--- a/KIK01接続一覧表.xlsx
+++ b/KIK01接続一覧表.xlsx
@@ -486,10 +486,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SyncOut</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>POTx8 LunchBox</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -801,7 +797,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2017.12.12</t>
+    <t>(SPI2_MISO)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2017.12.18</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -843,7 +843,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -934,8 +934,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -996,19 +1002,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1090,9 +1083,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -1153,7 +1143,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1678,7 +1671,7 @@
   <cols>
     <col min="1" max="1" width="2.25" customWidth="1"/>
     <col min="2" max="2" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.625" customWidth="1"/>
+    <col min="4" max="4" width="3.125" customWidth="1"/>
     <col min="6" max="6" width="10.375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="2.625" customWidth="1"/>
@@ -1713,7 +1706,7 @@
         <v>5</v>
       </c>
       <c r="Q5" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:24" s="5" customFormat="1">
@@ -1769,10 +1762,10 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F7" t="s">
         <v>182</v>
-      </c>
-      <c r="F7" t="s">
-        <v>183</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1781,10 +1774,10 @@
         <v>23</v>
       </c>
       <c r="O7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1918,17 +1911,14 @@
       <c r="M14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N14" s="13"/>
-      <c r="O14" s="13"/>
-      <c r="P14" s="30"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="Q14" s="18" t="s">
-        <v>28</v>
-      </c>
-      <c r="R14" s="2"/>
-      <c r="S14" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="T14" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -1948,13 +1938,13 @@
       </c>
       <c r="N15" s="13"/>
       <c r="O15" s="13"/>
-      <c r="P15" s="30"/>
+      <c r="P15" s="29"/>
       <c r="Q15" s="18" t="s">
         <v>29</v>
       </c>
       <c r="R15" s="13"/>
       <c r="S15" s="13"/>
-      <c r="T15" s="30"/>
+      <c r="T15" s="29"/>
     </row>
     <row r="16" spans="1:24">
       <c r="B16">
@@ -1964,10 +1954,10 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" t="s">
         <v>187</v>
-      </c>
-      <c r="F16" t="s">
-        <v>188</v>
       </c>
       <c r="G16" s="13"/>
       <c r="L16">
@@ -1976,17 +1966,14 @@
       <c r="M16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="P16" t="s">
+        <v>13</v>
+      </c>
       <c r="Q16" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="R16" s="12"/>
-      <c r="S16" s="25" t="s">
-        <v>85</v>
-      </c>
-      <c r="T16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2011,11 +1998,11 @@
         <v>13</v>
       </c>
       <c r="R17" s="12"/>
-      <c r="S17" s="25" t="s">
+      <c r="S17" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="T17" s="30" t="s">
         <v>140</v>
-      </c>
-      <c r="T17" s="31" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="18" spans="2:20">
@@ -2077,12 +2064,12 @@
       <c r="N20" s="13"/>
       <c r="O20" s="13"/>
       <c r="P20" s="13"/>
-      <c r="Q20" s="43" t="s">
+      <c r="Q20" s="42" t="s">
         <v>92</v>
       </c>
-      <c r="R20" s="26"/>
+      <c r="R20" s="25"/>
       <c r="S20" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="2:20">
@@ -2127,10 +2114,10 @@
         <v>94</v>
       </c>
       <c r="R22" s="6"/>
-      <c r="S22" s="25" t="s">
+      <c r="S22" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="T22" s="31" t="s">
+      <c r="T22" s="30" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2191,7 +2178,7 @@
         <v>37</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="2:20" s="5" customFormat="1">
@@ -2268,7 +2255,7 @@
       <c r="G30" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="I30" s="25" t="s">
+      <c r="I30" s="24" t="s">
         <v>116</v>
       </c>
       <c r="J30" s="13" t="s">
@@ -2296,7 +2283,7 @@
       <c r="G31" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="I31" s="25" t="s">
+      <c r="I31" s="24" t="s">
         <v>116</v>
       </c>
       <c r="J31" s="13" t="s">
@@ -2307,13 +2294,6 @@
       </c>
       <c r="M31" t="s">
         <v>58</v>
-      </c>
-      <c r="N31" s="2"/>
-      <c r="O31" t="s">
-        <v>192</v>
-      </c>
-      <c r="P31" t="s">
-        <v>193</v>
       </c>
       <c r="Q31" s="13"/>
       <c r="R31" s="13"/>
@@ -2347,18 +2327,15 @@
       <c r="C33" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="F33" t="s">
+        <v>83</v>
+      </c>
       <c r="G33" s="17" t="s">
         <v>13</v>
-      </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J33" t="s">
-        <v>83</v>
       </c>
       <c r="K33" s="13"/>
       <c r="L33">
@@ -2384,10 +2361,10 @@
         <v>100</v>
       </c>
       <c r="H34" s="8"/>
-      <c r="I34" s="25" t="s">
+      <c r="I34" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="J34" s="31" t="s">
+      <c r="J34" s="30" t="s">
         <v>88</v>
       </c>
       <c r="K34" s="13"/>
@@ -2397,12 +2374,12 @@
       <c r="M34" t="s">
         <v>60</v>
       </c>
-      <c r="N34" s="7"/>
+      <c r="N34" s="2"/>
       <c r="O34" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="Q34" s="13"/>
       <c r="R34" s="13"/>
@@ -2429,10 +2406,10 @@
       </c>
       <c r="N35" s="6"/>
       <c r="O35" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P35" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q35" s="13"/>
       <c r="R35" s="13"/>
@@ -2457,12 +2434,12 @@
       <c r="M36" t="s">
         <v>62</v>
       </c>
-      <c r="N36" s="8"/>
+      <c r="N36" s="7"/>
       <c r="O36" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q36" s="13"/>
       <c r="R36" s="13"/>
@@ -2480,7 +2457,7 @@
       <c r="G37" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="I37" s="25" t="s">
+      <c r="I37" s="24" t="s">
         <v>116</v>
       </c>
       <c r="J37" t="s">
@@ -2503,32 +2480,29 @@
       <c r="C38" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="32"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" t="s">
+        <v>84</v>
+      </c>
       <c r="G38" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J38" t="s">
-        <v>84</v>
-      </c>
-      <c r="K38" s="32"/>
+      <c r="K38" s="31"/>
       <c r="L38">
         <v>20</v>
       </c>
       <c r="M38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N38" s="29"/>
+      <c r="N38" s="28"/>
       <c r="O38" t="s">
+        <v>189</v>
+      </c>
+      <c r="P38" t="s">
         <v>190</v>
-      </c>
-      <c r="P38" t="s">
-        <v>191</v>
       </c>
       <c r="Q38" s="13"/>
       <c r="R38" s="13"/>
@@ -2540,18 +2514,15 @@
       <c r="C39" t="s">
         <v>47</v>
       </c>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" t="s">
+        <v>80</v>
+      </c>
       <c r="G39" s="19" t="s">
         <v>105</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J39" t="s">
-        <v>80</v>
       </c>
       <c r="K39" s="13"/>
       <c r="L39">
@@ -2560,6 +2531,13 @@
       <c r="M39" t="s">
         <v>63</v>
       </c>
+      <c r="N39" s="8"/>
+      <c r="O39" t="s">
+        <v>191</v>
+      </c>
+      <c r="P39" t="s">
+        <v>192</v>
+      </c>
       <c r="Q39" s="13"/>
       <c r="R39" s="13"/>
     </row>
@@ -2570,18 +2548,15 @@
       <c r="C40" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="D40" s="10"/>
+      <c r="E40" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F40" t="s">
+        <v>81</v>
+      </c>
       <c r="G40" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="H40" s="10"/>
-      <c r="I40" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J40" t="s">
-        <v>81</v>
       </c>
       <c r="K40" s="13"/>
       <c r="L40">
@@ -2600,18 +2575,15 @@
       <c r="C41" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F41" t="s">
+        <v>79</v>
+      </c>
       <c r="G41" s="19" t="s">
         <v>107</v>
-      </c>
-      <c r="H41" s="9"/>
-      <c r="I41" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J41" t="s">
-        <v>79</v>
       </c>
       <c r="K41" s="13"/>
       <c r="L41">
@@ -2637,18 +2609,15 @@
       <c r="C42" t="s">
         <v>50</v>
       </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
+      <c r="D42" s="8"/>
+      <c r="E42" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
       <c r="G42" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="H42" s="8"/>
-      <c r="I42" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J42" t="s">
-        <v>76</v>
       </c>
       <c r="K42" s="13"/>
       <c r="L42">
@@ -2657,6 +2626,9 @@
       <c r="M42" t="s">
         <v>65</v>
       </c>
+      <c r="P42" t="s">
+        <v>196</v>
+      </c>
       <c r="Q42" s="13"/>
       <c r="R42" s="13"/>
     </row>
@@ -2667,18 +2639,15 @@
       <c r="C43" t="s">
         <v>51</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" t="s">
+        <v>77</v>
+      </c>
       <c r="G43" s="19" t="s">
         <v>109</v>
-      </c>
-      <c r="H43" s="7"/>
-      <c r="I43" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J43" t="s">
-        <v>77</v>
       </c>
       <c r="K43" s="13"/>
       <c r="L43">
@@ -2704,18 +2673,15 @@
       <c r="C44" t="s">
         <v>52</v>
       </c>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F44" t="s">
+        <v>78</v>
+      </c>
       <c r="G44" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="H44" s="6"/>
-      <c r="I44" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="J44" t="s">
-        <v>78</v>
       </c>
       <c r="K44" s="13"/>
       <c r="L44">
@@ -2724,7 +2690,7 @@
       <c r="M44" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="N44" s="29"/>
+      <c r="N44" s="28"/>
       <c r="O44" t="s">
         <v>75</v>
       </c>
@@ -2747,16 +2713,14 @@
       <c r="G45" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="I45" s="25" t="s">
-        <v>119</v>
-      </c>
+      <c r="I45" s="13"/>
       <c r="L45">
         <v>34</v>
       </c>
       <c r="M45" t="s">
         <v>69</v>
       </c>
-      <c r="N45" s="33"/>
+      <c r="N45" s="32"/>
       <c r="O45" s="14" t="s">
         <v>75</v>
       </c>
@@ -2764,7 +2728,7 @@
         <v>74</v>
       </c>
       <c r="Q45" s="13"/>
-      <c r="R45" s="32"/>
+      <c r="R45" s="31"/>
       <c r="S45" s="14"/>
     </row>
     <row r="46" spans="2:19">
@@ -2794,7 +2758,7 @@
         <v>55</v>
       </c>
       <c r="D47" s="13"/>
-      <c r="G47" s="23" t="s">
+      <c r="G47" s="22" t="s">
         <v>113</v>
       </c>
       <c r="L47">
@@ -2810,21 +2774,21 @@
       <c r="Q48" s="13"/>
     </row>
     <row r="49" spans="3:17">
-      <c r="C49" s="24"/>
+      <c r="C49" s="23"/>
       <c r="D49" t="s">
         <v>114</v>
       </c>
       <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="3:17">
-      <c r="C50" s="31"/>
+      <c r="C50" s="30"/>
       <c r="D50" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="Q50" s="13"/>
     </row>
     <row r="51" spans="3:17">
-      <c r="C51" s="25"/>
+      <c r="C51" s="24"/>
       <c r="D51" t="s">
         <v>115</v>
       </c>
@@ -2850,20 +2814,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G109"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="7" max="7" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="B2" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="5" customFormat="1">
@@ -2883,27 +2850,27 @@
       </c>
       <c r="E4" s="2"/>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="E5" s="12"/>
+      <c r="E5" s="43"/>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="B6" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="5" customFormat="1">
@@ -2923,10 +2890,10 @@
       </c>
       <c r="E8" s="6"/>
       <c r="F8" t="s">
+        <v>124</v>
+      </c>
+      <c r="G8" t="s">
         <v>125</v>
-      </c>
-      <c r="G8" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -2935,10 +2902,10 @@
       </c>
       <c r="E9" s="8"/>
       <c r="F9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -2947,10 +2914,10 @@
       </c>
       <c r="E10" s="7"/>
       <c r="F10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -2959,10 +2926,10 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -2971,10 +2938,10 @@
       </c>
       <c r="E12" s="10"/>
       <c r="F12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.25" thickBot="1">
@@ -2983,39 +2950,39 @@
       </c>
       <c r="E13" s="11"/>
       <c r="F13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="14.25" thickBot="1">
       <c r="B14">
         <v>7</v>
       </c>
-      <c r="E14" s="26"/>
+      <c r="E14" s="25"/>
       <c r="F14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15">
         <v>8</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="26"/>
       <c r="F15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7">
-      <c r="B17" s="28" t="s">
-        <v>133</v>
+      <c r="B17" s="27" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1">
@@ -3035,10 +3002,10 @@
       </c>
       <c r="E19" s="6"/>
       <c r="F19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -3047,10 +3014,10 @@
       </c>
       <c r="E20" s="8"/>
       <c r="F20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -3059,10 +3026,10 @@
       </c>
       <c r="E21" s="7"/>
       <c r="F21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -3071,10 +3038,10 @@
       </c>
       <c r="E22" s="9"/>
       <c r="F22" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G22" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -3083,10 +3050,10 @@
       </c>
       <c r="E23" s="10"/>
       <c r="F23" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -3094,13 +3061,13 @@
         <v>6</v>
       </c>
       <c r="E24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F24" t="s">
+        <v>133</v>
+      </c>
+      <c r="G24" t="s">
         <v>134</v>
-      </c>
-      <c r="G24" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -3109,15 +3076,15 @@
       </c>
       <c r="E25" s="11"/>
       <c r="F25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1">
@@ -3135,12 +3102,12 @@
       <c r="B28">
         <v>1</v>
       </c>
-      <c r="E28" s="29"/>
+      <c r="E28" s="28"/>
       <c r="F28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -3149,20 +3116,20 @@
       </c>
       <c r="E29" s="2"/>
       <c r="F29" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:7" s="5" customFormat="1">
@@ -3182,10 +3149,10 @@
       </c>
       <c r="E34" s="6"/>
       <c r="F34" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="35" spans="1:7">
@@ -3194,10 +3161,10 @@
       </c>
       <c r="E35" s="8"/>
       <c r="F35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -3206,10 +3173,10 @@
       </c>
       <c r="E36" s="7"/>
       <c r="F36" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G36" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -3218,10 +3185,10 @@
       </c>
       <c r="E37" s="9"/>
       <c r="F37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -3230,10 +3197,10 @@
       </c>
       <c r="E38" s="10"/>
       <c r="F38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -3242,15 +3209,15 @@
       </c>
       <c r="E39" s="11"/>
       <c r="F39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="B40" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:7" s="5" customFormat="1">
@@ -3270,32 +3237,32 @@
       </c>
       <c r="E42" s="2"/>
       <c r="F42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="43" spans="1:7">
       <c r="B43">
         <v>2</v>
       </c>
-      <c r="E43" s="29"/>
+      <c r="E43" s="28"/>
       <c r="F43" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="A45" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="B46" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="47" spans="1:7" s="5" customFormat="1">
@@ -3315,10 +3282,10 @@
       </c>
       <c r="E48" s="6"/>
       <c r="F48" t="s">
+        <v>143</v>
+      </c>
+      <c r="G48" t="s">
         <v>144</v>
-      </c>
-      <c r="G48" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -3327,10 +3294,10 @@
       </c>
       <c r="E49" s="7"/>
       <c r="F49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -3339,27 +3306,27 @@
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="B51">
         <v>4</v>
       </c>
-      <c r="E51" s="29"/>
+      <c r="E51" s="28"/>
       <c r="F51" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G51" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:7">
       <c r="B52" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="14.25" thickBot="1">
@@ -3382,10 +3349,10 @@
       </c>
       <c r="E54" s="15"/>
       <c r="F54" t="s">
-        <v>151</v>
-      </c>
-      <c r="G54" s="31" t="s">
         <v>150</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -3394,10 +3361,10 @@
       </c>
       <c r="E55" s="12"/>
       <c r="F55" t="s">
+        <v>150</v>
+      </c>
+      <c r="G55" s="30" t="s">
         <v>151</v>
-      </c>
-      <c r="G55" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -3422,10 +3389,10 @@
       </c>
       <c r="E58" s="2"/>
       <c r="F58" t="s">
+        <v>152</v>
+      </c>
+      <c r="G58" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -3434,10 +3401,10 @@
       </c>
       <c r="E59" s="12"/>
       <c r="F59" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -3447,12 +3414,12 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="B62" s="5" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="63" spans="1:7" s="5" customFormat="1" ht="14.25" thickBot="1">
@@ -3472,10 +3439,10 @@
       </c>
       <c r="E64" s="15"/>
       <c r="F64" s="13" t="s">
-        <v>151</v>
-      </c>
-      <c r="G64" s="31" t="s">
         <v>150</v>
+      </c>
+      <c r="G64" s="30" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -3484,15 +3451,15 @@
       </c>
       <c r="E65" s="12"/>
       <c r="F65" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="G65" s="30" t="s">
         <v>151</v>
-      </c>
-      <c r="G65" s="31" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="B66" s="5" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1">
@@ -3512,10 +3479,10 @@
       </c>
       <c r="E68" s="13"/>
       <c r="F68" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="69" spans="1:7">
@@ -3523,16 +3490,16 @@
         <v>2</v>
       </c>
       <c r="E69" s="13"/>
-      <c r="F69" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="G69" s="32" t="s">
-        <v>161</v>
+      <c r="F69" s="31" t="s">
+        <v>160</v>
+      </c>
+      <c r="G69" s="31" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="B70" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="71" spans="1:7" s="5" customFormat="1">
@@ -3552,10 +3519,10 @@
       </c>
       <c r="E72" s="13"/>
       <c r="F72" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -3564,10 +3531,10 @@
       </c>
       <c r="E73" s="13"/>
       <c r="F73" s="13" t="s">
-        <v>161</v>
-      </c>
-      <c r="G73" s="32" t="s">
-        <v>161</v>
+        <v>160</v>
+      </c>
+      <c r="G73" s="31" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -3592,10 +3559,10 @@
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="14.25" thickBot="1">
@@ -3604,32 +3571,32 @@
       </c>
       <c r="E77" s="12"/>
       <c r="F77" t="s">
+        <v>177</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="14.25" thickBot="1">
       <c r="B78">
         <v>3</v>
       </c>
-      <c r="E78" s="26"/>
+      <c r="E78" s="25"/>
       <c r="F78" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="5" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="81" spans="2:7">
       <c r="B81" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="82" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
@@ -3644,15 +3611,15 @@
       </c>
     </row>
     <row r="83" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
-      <c r="B83" s="34">
+      <c r="B83" s="33">
         <v>1</v>
       </c>
-      <c r="E83" s="35"/>
-      <c r="F83" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="G83" s="39" t="s">
-        <v>150</v>
+      <c r="E83" s="34"/>
+      <c r="F83" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G83" s="38" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="84" spans="2:7">
@@ -3660,16 +3627,16 @@
         <v>2</v>
       </c>
       <c r="E84" s="12"/>
-      <c r="F84" s="34" t="s">
-        <v>160</v>
-      </c>
-      <c r="G84" s="31" t="s">
-        <v>152</v>
+      <c r="F84" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G84" s="30" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="85" spans="2:7">
       <c r="B85" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="86" spans="2:7" s="5" customFormat="1">
@@ -3684,31 +3651,31 @@
       </c>
     </row>
     <row r="87" spans="2:7" s="5" customFormat="1">
-      <c r="B87" s="34">
+      <c r="B87" s="33">
         <v>1</v>
       </c>
-      <c r="E87" s="37"/>
-      <c r="F87" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G87" s="39" t="s">
-        <v>165</v>
+      <c r="E87" s="36"/>
+      <c r="F87" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G87" s="38" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="88" spans="2:7">
       <c r="B88">
         <v>2</v>
       </c>
-      <c r="F88" s="36" t="s">
-        <v>161</v>
+      <c r="F88" s="35" t="s">
+        <v>160</v>
       </c>
       <c r="G88" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="89" spans="2:7">
       <c r="B89" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="90" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
@@ -3723,15 +3690,15 @@
       </c>
     </row>
     <row r="91" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
-      <c r="B91" s="34">
+      <c r="B91" s="33">
         <v>1</v>
       </c>
-      <c r="E91" s="38"/>
-      <c r="F91" s="34" t="s">
+      <c r="E91" s="37"/>
+      <c r="F91" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="G91" s="38" t="s">
         <v>162</v>
-      </c>
-      <c r="G91" s="39" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="92" spans="2:7">
@@ -3740,15 +3707,15 @@
       </c>
       <c r="E92" s="12"/>
       <c r="F92" t="s">
-        <v>162</v>
-      </c>
-      <c r="G92" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
+      </c>
+      <c r="G92" s="30" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="93" spans="2:7">
       <c r="B93" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="94" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
@@ -3763,15 +3730,15 @@
       </c>
     </row>
     <row r="95" spans="2:7" s="5" customFormat="1" ht="14.25" thickBot="1">
-      <c r="B95" s="34">
+      <c r="B95" s="33">
         <v>1</v>
       </c>
-      <c r="E95" s="42"/>
-      <c r="F95" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="G95" s="39" t="s">
-        <v>150</v>
+      <c r="E95" s="41"/>
+      <c r="F95" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G95" s="38" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="96" spans="2:7">
@@ -3779,16 +3746,16 @@
         <v>2</v>
       </c>
       <c r="E96" s="12"/>
-      <c r="F96" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="G96" s="31" t="s">
-        <v>152</v>
+      <c r="F96" s="33" t="s">
+        <v>168</v>
+      </c>
+      <c r="G96" s="30" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="97" spans="2:7">
       <c r="B97" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="2:7" s="5" customFormat="1">
@@ -3803,15 +3770,15 @@
       </c>
     </row>
     <row r="99" spans="2:7" s="5" customFormat="1">
-      <c r="B99" s="34">
+      <c r="B99" s="33">
         <v>1</v>
       </c>
-      <c r="E99" s="41"/>
-      <c r="F99" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G99" s="39" t="s">
-        <v>170</v>
+      <c r="E99" s="40"/>
+      <c r="F99" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G99" s="38" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="100" spans="2:7">
@@ -3819,16 +3786,16 @@
         <v>2</v>
       </c>
       <c r="E100" s="12"/>
-      <c r="F100" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="G100" s="31" t="s">
-        <v>171</v>
+      <c r="F100" s="33" t="s">
+        <v>143</v>
+      </c>
+      <c r="G100" s="30" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="2:7">
       <c r="B101" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="102" spans="2:7" s="5" customFormat="1">
@@ -3843,15 +3810,15 @@
       </c>
     </row>
     <row r="103" spans="2:7" s="5" customFormat="1">
-      <c r="B103" s="34">
+      <c r="B103" s="33">
         <v>1</v>
       </c>
-      <c r="E103" s="40"/>
-      <c r="F103" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="G103" s="39" t="s">
-        <v>172</v>
+      <c r="E103" s="39"/>
+      <c r="F103" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="G103" s="38" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="104" spans="2:7">
@@ -3860,10 +3827,10 @@
       </c>
       <c r="E104" s="12"/>
       <c r="F104" t="s">
-        <v>162</v>
-      </c>
-      <c r="G104" s="31" t="s">
-        <v>173</v>
+        <v>161</v>
+      </c>
+      <c r="G104" s="30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="105" spans="2:7">
@@ -3888,10 +3855,10 @@
       </c>
       <c r="E107" s="2"/>
       <c r="F107" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="108" spans="2:7" ht="14.25" thickBot="1">
@@ -3900,22 +3867,22 @@
       </c>
       <c r="E108" s="12"/>
       <c r="F108" t="s">
+        <v>177</v>
+      </c>
+      <c r="G108" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="109" spans="2:7" ht="14.25" thickBot="1">
       <c r="B109">
         <v>3</v>
       </c>
-      <c r="E109" s="26"/>
+      <c r="E109" s="25"/>
       <c r="F109" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>